<commit_message>
Correcting code with SonarLint(95/100)
</commit_message>
<xml_diff>
--- a/Docs/Lab01/Lab01_ReviewReport.xlsx
+++ b/Docs/Lab01/Lab01_ReviewReport.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rusu1\Desktop\VVSS\VVSS\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rusu1\Desktop\VVSS\VVSS\Docs\Lab01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6428454-99A4-4DAC-A292-EC777D5336B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E8D7615-F3FC-4F9D-B47D-500A929E8F73}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="650" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="80">
   <si>
     <t>Document  Title:</t>
   </si>
@@ -102,9 +102,6 @@
     <t>Student 3:</t>
   </si>
   <si>
-    <t>Echipa</t>
-  </si>
-  <si>
     <t>Grupa</t>
   </si>
   <si>
@@ -129,9 +126,6 @@
     <t>Numele si prenumele</t>
   </si>
   <si>
-    <t>Effort to perform dynamic code analysis (hours):</t>
-  </si>
-  <si>
     <t>R01</t>
   </si>
   <si>
@@ -199,19 +193,104 @@
   </si>
   <si>
     <t>Nu este indicat modul în care arată aplicația și nici tipul ei (web, desktop...).</t>
+  </si>
+  <si>
+    <t>Product.java, 139</t>
+  </si>
+  <si>
+    <t>Use isEmpty() to check whether the collection is empty or not</t>
+  </si>
+  <si>
+    <t xml:space="preserve">if (parts.size() &lt; 1) </t>
+  </si>
+  <si>
+    <t>if (parts.isEmpty())</t>
+  </si>
+  <si>
+    <t>Invetory.java, 53</t>
+  </si>
+  <si>
+    <t>Remove the literal "false" boolean value</t>
+  </si>
+  <si>
+    <t>if(isFound == false)</t>
+  </si>
+  <si>
+    <t>if(!isFound)</t>
+  </si>
+  <si>
+    <t>InvetoryRepository.java, 31, 82, 135</t>
+  </si>
+  <si>
+    <t>Use try-with-resources or close this "BufferdWriter" in a "finally" close</t>
+  </si>
+  <si>
+    <t>br = new BufferedReader(new FileReader(file));</t>
+  </si>
+  <si>
+    <t xml:space="preserve">try(BufferedReader br = new BufferedReader(new FileReader(file))) </t>
+  </si>
+  <si>
+    <t>AddPartController.java, 27</t>
+  </si>
+  <si>
+    <t>Remove this "String" constructor</t>
+  </si>
+  <si>
+    <t>private String errorMessage = new String();</t>
+  </si>
+  <si>
+    <t>private String errorMessage;</t>
+  </si>
+  <si>
+    <t>AddPartController.java, 108</t>
+  </si>
+  <si>
+    <t>Call "result.isPresent()" before accessing the value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        if(result.isPresent() &amp;&amp; result.get() == ButtonType.OK)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AddProductController.java, 153, 156, 175, 178, 222 </t>
+  </si>
+  <si>
+    <t>Replace this use of System.out or System.err by a logger</t>
+  </si>
+  <si>
+    <t>System.out.println("Part deleted.");</t>
+  </si>
+  <si>
+    <t>logger.info("Part deleted.");</t>
+  </si>
+  <si>
+    <t xml:space="preserve">if(result.get() == ButtonType.OK) </t>
+  </si>
+  <si>
+    <t>27.02.2020</t>
+  </si>
+  <si>
+    <t>Effort to perform dynamic code analysis (hours): 1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -390,81 +469,84 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -809,8 +891,8 @@
   </sheetPr>
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J5" sqref="I3:J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -831,7 +913,7 @@
         <v>3</v>
       </c>
       <c r="H1" s="23" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I1" s="24"/>
       <c r="J1" s="24"/>
@@ -845,10 +927,10 @@
       <c r="E2" s="25"/>
       <c r="H2" s="3"/>
       <c r="I2" s="20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J2" s="18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -856,7 +938,7 @@
         <v>20</v>
       </c>
       <c r="I3" s="21" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="J3" s="18">
         <v>236</v>
@@ -874,7 +956,7 @@
         <v>21</v>
       </c>
       <c r="I4" s="21" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J4" s="3">
         <v>236</v>
@@ -900,7 +982,7 @@
         <v>2</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E6" s="22"/>
     </row>
@@ -909,7 +991,7 @@
         <v>1</v>
       </c>
       <c r="D7" s="22" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E7" s="22"/>
     </row>
@@ -932,13 +1014,13 @@
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -947,13 +1029,13 @@
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
@@ -962,11 +1044,11 @@
         <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -975,11 +1057,11 @@
         <v>4</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
@@ -1121,8 +1203,8 @@
   </sheetPr>
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1141,8 +1223,8 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="24" t="s">
-        <v>23</v>
+      <c r="H1" s="37" t="s">
+        <v>50</v>
       </c>
       <c r="I1" s="24"/>
       <c r="J1" s="24"/>
@@ -1156,10 +1238,10 @@
       <c r="E2" s="25"/>
       <c r="H2" s="3"/>
       <c r="I2" s="20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J2" s="18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -1167,7 +1249,7 @@
         <v>20</v>
       </c>
       <c r="I3" s="21" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="J3" s="18">
         <v>236</v>
@@ -1185,7 +1267,7 @@
         <v>21</v>
       </c>
       <c r="I4" s="21" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J4" s="3">
         <v>236</v>
@@ -1211,7 +1293,7 @@
         <v>2</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E6" s="22"/>
     </row>
@@ -1220,7 +1302,7 @@
         <v>1</v>
       </c>
       <c r="D7" s="22" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E7" s="22"/>
     </row>
@@ -1243,11 +1325,11 @@
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
@@ -1256,11 +1338,11 @@
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -1269,11 +1351,11 @@
         <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
@@ -1282,11 +1364,11 @@
         <v>4</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
@@ -1295,11 +1377,11 @@
         <v>5</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
@@ -1442,7 +1524,7 @@
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="J5" sqref="I3:J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1462,8 +1544,8 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="24" t="s">
-        <v>23</v>
+      <c r="H1" s="37" t="s">
+        <v>50</v>
       </c>
       <c r="I1" s="24"/>
       <c r="J1" s="24"/>
@@ -1477,18 +1559,22 @@
       <c r="E2" s="25"/>
       <c r="H2" s="3"/>
       <c r="I2" s="20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J2" s="18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H3" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
+      <c r="I3" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="J3" s="18">
+        <v>236</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C4" s="17" t="s">
@@ -1501,8 +1587,12 @@
       <c r="H4" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
+      <c r="I4" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="J4" s="3">
+        <v>236</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C5" s="17" t="s">
@@ -1766,8 +1856,8 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1788,51 +1878,61 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="24" t="s">
-        <v>23</v>
+      <c r="H1" s="37" t="s">
+        <v>50</v>
       </c>
       <c r="I1" s="24"/>
       <c r="J1" s="24"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B2" s="25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C2" s="25"/>
       <c r="D2" s="25"/>
       <c r="E2" s="25"/>
       <c r="H2" s="3"/>
       <c r="I2" s="20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J2" s="18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H3" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
+      <c r="I3" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="J3" s="18">
+        <v>236</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C4" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D4" s="32"/>
       <c r="E4" s="32"/>
       <c r="H4" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
+      <c r="I4" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="J4" s="3">
+        <v>236</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="22"/>
+      <c r="D5" s="22" t="s">
+        <v>50</v>
+      </c>
       <c r="E5" s="22"/>
       <c r="H5" s="18" t="s">
         <v>22</v>
@@ -1845,7 +1945,9 @@
       <c r="C6" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="22"/>
+      <c r="D6" s="22" t="s">
+        <v>78</v>
+      </c>
       <c r="E6" s="22"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
@@ -1853,83 +1955,131 @@
         <v>4</v>
       </c>
       <c r="C9" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="F9" s="10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C10" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C11" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C12" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C13" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C14" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
+      <c r="C15" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C16" s="1"/>
+      <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
@@ -1939,7 +2089,7 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C17" s="1"/>
+      <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
@@ -1949,7 +2099,7 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C18" s="1"/>
+      <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
@@ -1959,8 +2109,8 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
     </row>
@@ -1969,7 +2119,7 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="C20" s="1"/>
+      <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
@@ -1979,8 +2129,8 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
     </row>
@@ -1989,7 +2139,7 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="C22" s="1"/>
+      <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
@@ -1999,7 +2149,7 @@
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="C23" s="1"/>
+      <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
@@ -2009,7 +2159,7 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="C24" s="1"/>
+      <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
@@ -2019,7 +2169,7 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="C25" s="1"/>
+      <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
@@ -2029,8 +2179,8 @@
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
     </row>
@@ -2039,17 +2189,17 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="C27" s="1"/>
+      <c r="C27" s="2"/>
       <c r="D27" s="2"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B28" s="3">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="C28" s="1"/>
+      <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
@@ -2059,7 +2209,7 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="C29" s="1"/>
+      <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
@@ -2069,7 +2219,7 @@
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="C30" s="1"/>
+      <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
@@ -2079,7 +2229,7 @@
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C32" s="35" t="s">
-        <v>32</v>
+        <v>79</v>
       </c>
       <c r="D32" s="36"/>
       <c r="E32" s="36"/>

</xml_diff>

<commit_message>
Review Coding Phase & Update Code
</commit_message>
<xml_diff>
--- a/Docs/Lab01/Lab01_ReviewReport.xlsx
+++ b/Docs/Lab01/Lab01_ReviewReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rusu1\Desktop\VVSS\VVSS\Docs\Lab01\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pigeon\Documents\facultate\An3\VVSS\Inventory\Docs\Lab01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FA87F46-911E-4BE3-BBAE-BA6C87EF3CF5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FB98486-2B10-4CBA-9D8B-CC8FB4CEF3B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="650" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="650" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Coding Phase Defects" sheetId="5" r:id="rId3"/>
     <sheet name="DynamicCodeAnalysis" sheetId="8" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="102">
   <si>
     <t>Document  Title:</t>
   </si>
@@ -285,15 +285,9 @@
     <t>public void updateInhousePart(int partIndex, int partId, String name, double price, int inStock, int min, int max, int partDynamicValue)</t>
   </si>
   <si>
-    <t>AddPartController.java, 173</t>
-  </si>
-  <si>
     <t>Se afișează următorul mesaj: "Form contains blank field." în momentul în care se încearcă salvarea unor date greșite (tipul diferă, în loc de int se introduce string). Ar trebui afișat un mesaj corespunzător problemei.</t>
   </si>
   <si>
-    <t>ModifyPartController.java, 78</t>
-  </si>
-  <si>
     <t>ModifyPartController.java, 139</t>
   </si>
   <si>
@@ -304,19 +298,65 @@
   </si>
   <si>
     <t>Daca nu se selecteză o piesă pentru ștergere în interfața cu utilizatorul ar trebui să apară un mesaj prin care să fie atenționat că este necesar să selecteze o piesă. În momentul de față, nu apare nimic pe interfață, dar se aruncă o eroare (java.lang.NullPointerException), deoarece nu se verifică dacă a fost selectată o piesă și se încearcă apelarea metodei getName() pe o piesă cu valoarea null.</t>
+  </si>
+  <si>
+    <t>C01</t>
+  </si>
+  <si>
+    <t>Part.java, 93</t>
+  </si>
+  <si>
+    <t>InventoryRepository.java, 26, 73, 121</t>
+  </si>
+  <si>
+    <t>C08</t>
+  </si>
+  <si>
+    <t>C06</t>
+  </si>
+  <si>
+    <t>MainScreenController.java, 210,223,158,128</t>
+  </si>
+  <si>
+    <t>Variabila inStock e comparată cu 1 în loc de 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dacă fisierul cu date nu există în resurse, aplicația va arunca NullPointerException. Ar trebui reținut rezultatul apelării getResource, și comparat cu null, dacă este cazul aruncată o eroare adecvată </t>
+  </si>
+  <si>
+    <t>La operațiile de modificare și ștergere, în interfața cu utilizatorul ar trebui să apară un mesaj prin care să fie atenționat că este necesar să selecteze un obiect, in momentul de față, dacă un obiect nu e selectat, valoarea va fi null si se continua cu null în funcțiile urmatoare</t>
+  </si>
+  <si>
+    <t>AddPartController.java, 166; AddProductController.java, 212; ModifyPartController.java, 193; ModifyProductController.java, 236</t>
+  </si>
+  <si>
+    <t>MainScreenController.java, 185,187</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pentru metoda String.format se folosește "{}" in loc de "%s" </t>
+  </si>
+  <si>
+    <t>C04</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -502,84 +542,90 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -928,36 +974,36 @@
       <selection activeCell="J5" sqref="I3:J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="6"/>
-    <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
-    <col min="3" max="4" width="16.33203125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="41.44140625" style="6" customWidth="1"/>
-    <col min="6" max="8" width="8.88671875" style="6"/>
+    <col min="1" max="1" width="8.85546875" style="6"/>
+    <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
+    <col min="3" max="4" width="16.28515625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="41.42578125" style="6" customWidth="1"/>
+    <col min="6" max="8" width="8.85546875" style="6"/>
     <col min="9" max="9" width="21" style="6" customWidth="1"/>
-    <col min="10" max="10" width="14.44140625" style="6" customWidth="1"/>
-    <col min="11" max="16384" width="8.88671875" style="6"/>
+    <col min="10" max="10" width="14.42578125" style="6" customWidth="1"/>
+    <col min="11" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B2" s="25" t="s">
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B2" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
       <c r="H2" s="3"/>
       <c r="I2" s="20" t="s">
         <v>30</v>
@@ -966,7 +1012,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H3" s="18" t="s">
         <v>20</v>
       </c>
@@ -977,14 +1023,14 @@
         <v>236</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C4" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="26" t="s">
+      <c r="D4" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="26"/>
+      <c r="E4" s="27"/>
       <c r="H4" s="18" t="s">
         <v>21</v>
       </c>
@@ -995,40 +1041,40 @@
         <v>236</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C5" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="27" t="s">
+      <c r="D5" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="28"/>
+      <c r="E5" s="29"/>
       <c r="H5" s="18" t="s">
         <v>22</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="22" t="s">
+      <c r="D6" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="E6" s="22"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E6" s="23"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="22" t="s">
+      <c r="D7" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="E7" s="22"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E7" s="23"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -1042,7 +1088,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -1056,7 +1102,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
@@ -1071,7 +1117,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B25" si="0">B11+1</f>
         <v>3</v>
@@ -1084,7 +1130,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1097,7 +1143,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1106,7 +1152,7 @@
       <c r="D14" s="1"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1115,7 +1161,7 @@
       <c r="D15" s="1"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1124,7 +1170,7 @@
       <c r="D16" s="1"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1133,7 +1179,7 @@
       <c r="D17" s="1"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1142,7 +1188,7 @@
       <c r="D18" s="3"/>
       <c r="E18" s="16"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1151,7 +1197,7 @@
       <c r="D19" s="3"/>
       <c r="E19" s="16"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1160,7 +1206,7 @@
       <c r="D20" s="3"/>
       <c r="E20" s="16"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1169,7 +1215,7 @@
       <c r="D21" s="3"/>
       <c r="E21" s="16"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1178,7 +1224,7 @@
       <c r="D22" s="3"/>
       <c r="E22" s="16"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1187,7 +1233,7 @@
       <c r="D23" s="3"/>
       <c r="E23" s="16"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1196,7 +1242,7 @@
       <c r="D24" s="3"/>
       <c r="E24" s="16"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1205,10 +1251,10 @@
       <c r="D25" s="3"/>
       <c r="E25" s="16"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E26" s="11"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C27" s="12" t="s">
         <v>8</v>
       </c>
@@ -1236,39 +1282,39 @@
   </sheetPr>
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="H1" sqref="H1:J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="6"/>
-    <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
-    <col min="3" max="4" width="16.33203125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="41.44140625" style="6" customWidth="1"/>
-    <col min="6" max="8" width="8.88671875" style="6"/>
+    <col min="1" max="1" width="8.85546875" style="6"/>
+    <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
+    <col min="3" max="4" width="16.28515625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="41.42578125" style="6" customWidth="1"/>
+    <col min="6" max="8" width="8.85546875" style="6"/>
     <col min="9" max="9" width="22" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="6"/>
+    <col min="10" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="29" t="s">
+      <c r="H1" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B2" s="25" t="s">
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B2" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
       <c r="H2" s="3"/>
       <c r="I2" s="20" t="s">
         <v>30</v>
@@ -1277,7 +1323,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H3" s="18" t="s">
         <v>20</v>
       </c>
@@ -1288,14 +1334,14 @@
         <v>236</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="30" t="s">
+      <c r="D4" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="30"/>
+      <c r="E4" s="31"/>
       <c r="H4" s="18" t="s">
         <v>21</v>
       </c>
@@ -1306,40 +1352,40 @@
         <v>236</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="31" t="s">
+      <c r="D5" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="32"/>
+      <c r="E5" s="33"/>
       <c r="H5" s="18" t="s">
         <v>22</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="22" t="s">
+      <c r="D6" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="E6" s="22"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E6" s="23"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="22" t="s">
+      <c r="D7" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="E7" s="22"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E7" s="23"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -1353,7 +1399,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -1365,7 +1411,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
@@ -1378,7 +1424,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B26" si="0">B11+1</f>
         <v>3</v>
@@ -1391,7 +1437,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1404,7 +1450,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1417,7 +1463,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1426,7 +1472,7 @@
       <c r="D15" s="1"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1435,7 +1481,7 @@
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1444,7 +1490,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1453,7 +1499,7 @@
       <c r="D18" s="1"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1462,7 +1508,7 @@
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1471,7 +1517,7 @@
       <c r="D20" s="1"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1480,7 +1526,7 @@
       <c r="D21" s="1"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1489,7 +1535,7 @@
       <c r="D22" s="1"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1498,7 +1544,7 @@
       <c r="D23" s="1"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1507,7 +1553,7 @@
       <c r="D24" s="1"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1516,7 +1562,7 @@
       <c r="D25" s="1"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1525,10 +1571,10 @@
       <c r="D26" s="1"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E27" s="11"/>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C28" s="12" t="s">
         <v>8</v>
       </c>
@@ -1556,40 +1602,41 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E53" sqref="E53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="6"/>
-    <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="18" style="6" customWidth="1"/>
-    <col min="5" max="5" width="41.44140625" style="6" customWidth="1"/>
-    <col min="6" max="8" width="8.88671875" style="6"/>
-    <col min="9" max="9" width="26.6640625" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="6"/>
+    <col min="1" max="1" width="8.85546875" style="6"/>
+    <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="25" style="6" customWidth="1"/>
+    <col min="5" max="5" width="41.42578125" style="6" customWidth="1"/>
+    <col min="6" max="6" width="37.7109375" style="6" customWidth="1"/>
+    <col min="7" max="8" width="8.85546875" style="6"/>
+    <col min="9" max="9" width="26.7109375" style="6" customWidth="1"/>
+    <col min="10" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="29" t="s">
+      <c r="H1" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B2" s="25" t="s">
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B2" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
       <c r="H2" s="3"/>
       <c r="I2" s="20" t="s">
         <v>30</v>
@@ -1598,7 +1645,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H3" s="18" t="s">
         <v>20</v>
       </c>
@@ -1609,14 +1656,14 @@
         <v>236</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C4" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="33" t="s">
+      <c r="D4" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="33"/>
+      <c r="E4" s="34"/>
       <c r="H4" s="18" t="s">
         <v>21</v>
       </c>
@@ -1627,40 +1674,40 @@
         <v>236</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C5" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="34" t="s">
+      <c r="D5" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="35"/>
+      <c r="E5" s="36"/>
       <c r="H5" s="18" t="s">
         <v>22</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="22" t="s">
+      <c r="D6" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="E6" s="22"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E6" s="23"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="22" t="s">
-        <v>89</v>
-      </c>
-      <c r="E7" s="22"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D7" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="E7" s="23"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -1674,81 +1721,112 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="2"/>
+      <c r="C10" s="2" t="s">
+        <v>92</v>
+      </c>
       <c r="D10" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:10" ht="150" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="2"/>
+      <c r="C11" s="2" t="s">
+        <v>93</v>
+      </c>
       <c r="D11" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="F11" s="22"/>
+    </row>
+    <row r="12" spans="1:10" ht="150" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="2"/>
+      <c r="C12" s="2" t="s">
+        <v>93</v>
+      </c>
       <c r="D12" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E12" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="3">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B13" s="3">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E13" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C14" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C15" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E15" s="39" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C16" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E16" s="39" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1757,7 +1835,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1766,7 +1844,7 @@
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1775,7 +1853,7 @@
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1784,7 +1862,7 @@
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1793,7 +1871,7 @@
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1802,7 +1880,7 @@
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1811,7 +1889,7 @@
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1820,7 +1898,7 @@
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1829,7 +1907,7 @@
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1838,7 +1916,7 @@
       <c r="D26" s="1"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" s="3">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1847,7 +1925,7 @@
       <c r="D27" s="2"/>
       <c r="E27" s="1"/>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" s="3">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1856,7 +1934,7 @@
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" s="3">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1865,7 +1943,7 @@
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" s="3">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1874,10 +1952,10 @@
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E31" s="11"/>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C32" s="12" t="s">
         <v>8</v>
       </c>
@@ -1905,41 +1983,41 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
+    <sheetView topLeftCell="A8" workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="6"/>
-    <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" style="6" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="6"/>
+    <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" style="6" customWidth="1"/>
     <col min="4" max="4" width="18" style="6" customWidth="1"/>
     <col min="5" max="5" width="24" style="6" customWidth="1"/>
-    <col min="6" max="6" width="16.6640625" style="6" customWidth="1"/>
-    <col min="7" max="8" width="8.88671875" style="6"/>
-    <col min="9" max="9" width="26.6640625" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="6"/>
+    <col min="6" max="6" width="16.7109375" style="6" customWidth="1"/>
+    <col min="7" max="8" width="8.85546875" style="6"/>
+    <col min="9" max="9" width="26.7109375" style="6" customWidth="1"/>
+    <col min="10" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="29" t="s">
+      <c r="H1" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B2" s="25" t="s">
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B2" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
       <c r="H2" s="3"/>
       <c r="I2" s="20" t="s">
         <v>30</v>
@@ -1948,7 +2026,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H3" s="18" t="s">
         <v>20</v>
       </c>
@@ -1959,12 +2037,12 @@
         <v>236</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C4" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
       <c r="H4" s="18" t="s">
         <v>21</v>
       </c>
@@ -1975,31 +2053,31 @@
         <v>236</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="22" t="s">
+      <c r="D5" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="E5" s="22"/>
+      <c r="E5" s="23"/>
       <c r="H5" s="18" t="s">
         <v>22</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="22" t="s">
+      <c r="D6" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="E6" s="22"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E6" s="23"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -2016,7 +2094,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -2033,7 +2111,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
@@ -2051,7 +2129,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
@@ -2069,7 +2147,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -2087,7 +2165,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -2105,7 +2183,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -2123,7 +2201,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -2141,7 +2219,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -2151,7 +2229,7 @@
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -2161,7 +2239,7 @@
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -2171,7 +2249,7 @@
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -2181,7 +2259,7 @@
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -2191,7 +2269,7 @@
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -2201,7 +2279,7 @@
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -2211,7 +2289,7 @@
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -2221,7 +2299,7 @@
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -2231,7 +2309,7 @@
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -2241,7 +2319,7 @@
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27" s="3">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -2251,7 +2329,7 @@
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28" s="3">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -2261,7 +2339,7 @@
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B29" s="3">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -2271,7 +2349,7 @@
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B30" s="3">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -2281,15 +2359,15 @@
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E31" s="11"/>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C32" s="36" t="s">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C32" s="37" t="s">
         <v>79</v>
       </c>
-      <c r="D32" s="37"/>
-      <c r="E32" s="37"/>
+      <c r="D32" s="38"/>
+      <c r="E32" s="38"/>
       <c r="F32" s="19"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SonarLint update + ReviewReport modifed + Correct code
</commit_message>
<xml_diff>
--- a/Docs/Lab01/Lab01_ReviewReport.xlsx
+++ b/Docs/Lab01/Lab01_ReviewReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pigeon\Documents\facultate\An3\VVSS\Inventory\Docs\Lab01\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rusu1\Desktop\VVSS\VVSS\Docs\Lab01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FB98486-2B10-4CBA-9D8B-CC8FB4CEF3B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBAB1658-9E99-46AA-A26D-F8A649D2D19B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="650" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Coding Phase Defects" sheetId="5" r:id="rId3"/>
     <sheet name="DynamicCodeAnalysis" sheetId="8" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="99">
   <si>
     <t>Document  Title:</t>
   </si>
@@ -318,25 +318,16 @@
     <t>MainScreenController.java, 210,223,158,128</t>
   </si>
   <si>
-    <t>Variabila inStock e comparată cu 1 în loc de 0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dacă fisierul cu date nu există în resurse, aplicația va arunca NullPointerException. Ar trebui reținut rezultatul apelării getResource, și comparat cu null, dacă este cazul aruncată o eroare adecvată </t>
-  </si>
-  <si>
-    <t>La operațiile de modificare și ștergere, în interfața cu utilizatorul ar trebui să apară un mesaj prin care să fie atenționat că este necesar să selecteze un obiect, in momentul de față, dacă un obiect nu e selectat, valoarea va fi null si se continua cu null în funcțiile urmatoare</t>
-  </si>
-  <si>
     <t>AddPartController.java, 166; AddProductController.java, 212; ModifyPartController.java, 193; ModifyProductController.java, 236</t>
   </si>
   <si>
-    <t>MainScreenController.java, 185,187</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pentru metoda String.format se folosește "{}" in loc de "%s" </t>
-  </si>
-  <si>
-    <t>C04</t>
+    <t>Variabila inStock e comparată cu 1 în loc de 0.</t>
+  </si>
+  <si>
+    <t>Dacă fisierul cu date nu există în resurse, aplicația va arunca NullPointerException. Ar trebui reținut rezultatul apelării getResource, și comparat cu null, dacă este cazul aruncată o eroare adecvată.</t>
+  </si>
+  <si>
+    <t>La operațiile de modificare și ștergere, în interfața cu utilizatorul ar trebui să apară un mesaj prin care să fie atenționat că este necesar să selecteze un obiect, in momentul de față, dacă un obiect nu e selectat, valoarea va fi null si se continua cu null în funcțiile urmatoare.</t>
   </si>
 </sst>
 </file>
@@ -624,7 +615,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -970,23 +961,23 @@
   </sheetPr>
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J5" sqref="I3:J5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="6"/>
-    <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
-    <col min="3" max="4" width="16.28515625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="41.42578125" style="6" customWidth="1"/>
-    <col min="6" max="8" width="8.85546875" style="6"/>
+    <col min="1" max="1" width="8.88671875" style="6"/>
+    <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
+    <col min="3" max="4" width="16.33203125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="41.44140625" style="6" customWidth="1"/>
+    <col min="6" max="8" width="8.88671875" style="6"/>
     <col min="9" max="9" width="21" style="6" customWidth="1"/>
-    <col min="10" max="10" width="14.42578125" style="6" customWidth="1"/>
-    <col min="11" max="16384" width="8.85546875" style="6"/>
+    <col min="10" max="10" width="14.44140625" style="6" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
@@ -997,7 +988,7 @@
       <c r="I1" s="25"/>
       <c r="J1" s="25"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B2" s="26" t="s">
         <v>19</v>
       </c>
@@ -1012,7 +1003,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H3" s="18" t="s">
         <v>20</v>
       </c>
@@ -1023,7 +1014,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C4" s="14" t="s">
         <v>0</v>
       </c>
@@ -1041,7 +1032,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C5" s="14" t="s">
         <v>9</v>
       </c>
@@ -1055,7 +1046,7 @@
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
@@ -1065,7 +1056,7 @@
       </c>
       <c r="E6" s="23"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
@@ -1074,7 +1065,7 @@
       </c>
       <c r="E7" s="23"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -1088,7 +1079,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -1102,7 +1093,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
@@ -1117,7 +1108,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B25" si="0">B11+1</f>
         <v>3</v>
@@ -1130,7 +1121,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1143,7 +1134,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1152,7 +1143,7 @@
       <c r="D14" s="1"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1161,7 +1152,7 @@
       <c r="D15" s="1"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1170,7 +1161,7 @@
       <c r="D16" s="1"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1179,7 +1170,7 @@
       <c r="D17" s="1"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1188,7 +1179,7 @@
       <c r="D18" s="3"/>
       <c r="E18" s="16"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1197,7 +1188,7 @@
       <c r="D19" s="3"/>
       <c r="E19" s="16"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1206,7 +1197,7 @@
       <c r="D20" s="3"/>
       <c r="E20" s="16"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1215,7 +1206,7 @@
       <c r="D21" s="3"/>
       <c r="E21" s="16"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1224,7 +1215,7 @@
       <c r="D22" s="3"/>
       <c r="E22" s="16"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1233,7 +1224,7 @@
       <c r="D23" s="3"/>
       <c r="E23" s="16"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1242,7 +1233,7 @@
       <c r="D24" s="3"/>
       <c r="E24" s="16"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1251,15 +1242,17 @@
       <c r="D25" s="3"/>
       <c r="E25" s="16"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
       <c r="E26" s="11"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C27" s="12" t="s">
         <v>8</v>
       </c>
       <c r="D27" s="13"/>
-      <c r="E27" s="1"/>
+      <c r="E27" s="1">
+        <v>0.5</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1282,22 +1275,22 @@
   </sheetPr>
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="H1" sqref="H1:J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="6"/>
-    <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
-    <col min="3" max="4" width="16.28515625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="41.42578125" style="6" customWidth="1"/>
-    <col min="6" max="8" width="8.85546875" style="6"/>
+    <col min="1" max="1" width="8.88671875" style="6"/>
+    <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
+    <col min="3" max="4" width="16.33203125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="41.44140625" style="6" customWidth="1"/>
+    <col min="6" max="8" width="8.88671875" style="6"/>
     <col min="9" max="9" width="22" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="8.85546875" style="6"/>
+    <col min="10" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
@@ -1308,7 +1301,7 @@
       <c r="I1" s="25"/>
       <c r="J1" s="25"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B2" s="26" t="s">
         <v>18</v>
       </c>
@@ -1323,7 +1316,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H3" s="18" t="s">
         <v>20</v>
       </c>
@@ -1334,7 +1327,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C4" s="7" t="s">
         <v>0</v>
       </c>
@@ -1352,7 +1345,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C5" s="7" t="s">
         <v>10</v>
       </c>
@@ -1366,7 +1359,7 @@
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
@@ -1376,7 +1369,7 @@
       </c>
       <c r="E6" s="23"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
@@ -1385,7 +1378,7 @@
       </c>
       <c r="E7" s="23"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -1399,7 +1392,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -1411,7 +1404,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
@@ -1424,7 +1417,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B26" si="0">B11+1</f>
         <v>3</v>
@@ -1437,7 +1430,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1450,7 +1443,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="105" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1463,7 +1456,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1472,7 +1465,7 @@
       <c r="D15" s="1"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1481,7 +1474,7 @@
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1490,7 +1483,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1499,7 +1492,7 @@
       <c r="D18" s="1"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1508,7 +1501,7 @@
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1517,7 +1510,7 @@
       <c r="D20" s="1"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1526,7 +1519,7 @@
       <c r="D21" s="1"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1535,7 +1528,7 @@
       <c r="D22" s="1"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1544,7 +1537,7 @@
       <c r="D23" s="1"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1553,7 +1546,7 @@
       <c r="D24" s="1"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1562,7 +1555,7 @@
       <c r="D25" s="1"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1571,10 +1564,10 @@
       <c r="D26" s="1"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
       <c r="E27" s="11"/>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C28" s="12" t="s">
         <v>8</v>
       </c>
@@ -1602,24 +1595,24 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E53" sqref="E53"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="6"/>
-    <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" style="6" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" style="6"/>
+    <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" style="6" customWidth="1"/>
     <col min="4" max="4" width="25" style="6" customWidth="1"/>
-    <col min="5" max="5" width="41.42578125" style="6" customWidth="1"/>
-    <col min="6" max="6" width="37.7109375" style="6" customWidth="1"/>
-    <col min="7" max="8" width="8.85546875" style="6"/>
-    <col min="9" max="9" width="26.7109375" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="8.85546875" style="6"/>
+    <col min="5" max="5" width="41.44140625" style="6" customWidth="1"/>
+    <col min="6" max="6" width="37.6640625" style="6" customWidth="1"/>
+    <col min="7" max="8" width="8.88671875" style="6"/>
+    <col min="9" max="9" width="26.6640625" style="6" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
@@ -1630,7 +1623,7 @@
       <c r="I1" s="25"/>
       <c r="J1" s="25"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B2" s="26" t="s">
         <v>17</v>
       </c>
@@ -1645,7 +1638,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H3" s="18" t="s">
         <v>20</v>
       </c>
@@ -1656,7 +1649,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C4" s="17" t="s">
         <v>0</v>
       </c>
@@ -1674,7 +1667,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C5" s="17" t="s">
         <v>9</v>
       </c>
@@ -1688,7 +1681,7 @@
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
@@ -1698,7 +1691,7 @@
       </c>
       <c r="E6" s="23"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
@@ -1707,7 +1700,7 @@
       </c>
       <c r="E7" s="23"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -1721,7 +1714,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="120" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -1729,122 +1722,116 @@
         <v>92</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="150" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="39" t="s">
         <v>93</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>86</v>
+      <c r="D11" s="39" t="s">
+        <v>94</v>
+      </c>
+      <c r="E11" s="39" t="s">
+        <v>98</v>
       </c>
       <c r="F11" s="22"/>
     </row>
-    <row r="12" spans="1:10" ht="150" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="39" t="s">
         <v>93</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="39" t="s">
         <v>85</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E12" s="39" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="B13" s="3">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="C13" s="39" t="s">
+        <v>93</v>
+      </c>
+      <c r="D13" s="39" t="s">
+        <v>85</v>
+      </c>
+      <c r="E13" s="39" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="3">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="C13" s="2" t="s">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B14" s="3">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C14" s="39" t="s">
         <v>89</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D14" s="39" t="s">
         <v>90</v>
       </c>
-      <c r="E13" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="B14" s="3">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="D14" s="2" t="s">
+      <c r="E14" s="39" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+      <c r="B15" s="3">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="C15" s="39" t="s">
+        <v>93</v>
+      </c>
+      <c r="D15" s="39" t="s">
         <v>91</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="105" x14ac:dyDescent="0.25">
-      <c r="B15" s="3">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>94</v>
       </c>
       <c r="E15" s="39" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="E16" s="39" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C16" s="39"/>
+      <c r="D16" s="39"/>
+      <c r="E16" s="39"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C17" s="39"/>
+      <c r="D17" s="39"/>
+      <c r="E17" s="39"/>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C18" s="39"/>
+      <c r="D18" s="39"/>
+      <c r="E18" s="39"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1853,7 +1840,7 @@
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1862,7 +1849,7 @@
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1871,7 +1858,7 @@
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1880,7 +1867,7 @@
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1889,7 +1876,7 @@
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1898,7 +1885,7 @@
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1907,7 +1894,7 @@
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1916,7 +1903,7 @@
       <c r="D26" s="1"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B27" s="3">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1925,7 +1912,7 @@
       <c r="D27" s="2"/>
       <c r="E27" s="1"/>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B28" s="3">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1934,7 +1921,7 @@
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B29" s="3">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1943,7 +1930,7 @@
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B30" s="3">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1952,15 +1939,17 @@
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
       <c r="E31" s="11"/>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C32" s="12" t="s">
         <v>8</v>
       </c>
       <c r="D32" s="13"/>
-      <c r="E32" s="1"/>
+      <c r="E32" s="1">
+        <v>0.5</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1983,24 +1972,24 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
+    <sheetView topLeftCell="A15" workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="6"/>
-    <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" style="6" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" style="6"/>
+    <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" style="6" customWidth="1"/>
     <col min="4" max="4" width="18" style="6" customWidth="1"/>
     <col min="5" max="5" width="24" style="6" customWidth="1"/>
-    <col min="6" max="6" width="16.7109375" style="6" customWidth="1"/>
-    <col min="7" max="8" width="8.85546875" style="6"/>
-    <col min="9" max="9" width="26.7109375" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="8.85546875" style="6"/>
+    <col min="6" max="6" width="16.6640625" style="6" customWidth="1"/>
+    <col min="7" max="8" width="8.88671875" style="6"/>
+    <col min="9" max="9" width="26.6640625" style="6" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
@@ -2011,7 +2000,7 @@
       <c r="I1" s="25"/>
       <c r="J1" s="25"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B2" s="26" t="s">
         <v>24</v>
       </c>
@@ -2026,7 +2015,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H3" s="18" t="s">
         <v>20</v>
       </c>
@@ -2037,7 +2026,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C4" s="17" t="s">
         <v>25</v>
       </c>
@@ -2053,7 +2042,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C5" s="9" t="s">
         <v>2</v>
       </c>
@@ -2067,7 +2056,7 @@
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>1</v>
@@ -2077,7 +2066,7 @@
       </c>
       <c r="E6" s="23"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -2094,7 +2083,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -2111,7 +2100,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
@@ -2129,7 +2118,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
@@ -2147,7 +2136,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -2165,7 +2154,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -2183,7 +2172,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -2201,7 +2190,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="105" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -2219,7 +2208,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -2229,7 +2218,7 @@
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -2239,7 +2228,7 @@
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -2249,7 +2238,7 @@
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -2259,7 +2248,7 @@
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -2269,7 +2258,7 @@
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -2279,7 +2268,7 @@
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -2289,7 +2278,7 @@
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -2299,7 +2288,7 @@
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -2309,7 +2298,7 @@
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -2319,7 +2308,7 @@
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B27" s="3">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -2329,7 +2318,7 @@
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B28" s="3">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -2339,7 +2328,7 @@
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B29" s="3">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -2349,7 +2338,7 @@
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B30" s="3">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -2359,10 +2348,10 @@
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:6" x14ac:dyDescent="0.3">
       <c r="E31" s="11"/>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C32" s="37" t="s">
         <v>79</v>
       </c>

</xml_diff>

<commit_message>
Added error if repo file does not exist + Finished Review + Rename Files
</commit_message>
<xml_diff>
--- a/Docs/Lab01/Lab01_ReviewReport.xlsx
+++ b/Docs/Lab01/Lab01_ReviewReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rusu1\Desktop\VVSS\VVSS\Docs\Lab01\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pigeon\Documents\facultate\An3\VVSS\Inventory\Docs\Lab01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBAB1658-9E99-46AA-A26D-F8A649D2D19B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D976A8D-D4D1-43C0-83C5-CF9CC8BE6919}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Coding Phase Defects" sheetId="5" r:id="rId3"/>
     <sheet name="DynamicCodeAnalysis" sheetId="8" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -567,6 +567,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -614,9 +617,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -961,40 +961,40 @@
   </sheetPr>
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="6"/>
-    <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
-    <col min="3" max="4" width="16.33203125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="41.44140625" style="6" customWidth="1"/>
-    <col min="6" max="8" width="8.88671875" style="6"/>
+    <col min="1" max="1" width="8.85546875" style="6"/>
+    <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
+    <col min="3" max="4" width="16.28515625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="41.42578125" style="6" customWidth="1"/>
+    <col min="6" max="8" width="8.85546875" style="6"/>
     <col min="9" max="9" width="21" style="6" customWidth="1"/>
-    <col min="10" max="10" width="14.44140625" style="6" customWidth="1"/>
-    <col min="11" max="16384" width="8.88671875" style="6"/>
+    <col min="10" max="10" width="14.42578125" style="6" customWidth="1"/>
+    <col min="11" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="24" t="s">
+      <c r="H1" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B2" s="26" t="s">
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B2" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
       <c r="H2" s="3"/>
       <c r="I2" s="20" t="s">
         <v>30</v>
@@ -1003,7 +1003,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H3" s="18" t="s">
         <v>20</v>
       </c>
@@ -1014,14 +1014,14 @@
         <v>236</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C4" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="27" t="s">
+      <c r="D4" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="27"/>
+      <c r="E4" s="28"/>
       <c r="H4" s="18" t="s">
         <v>21</v>
       </c>
@@ -1032,40 +1032,40 @@
         <v>236</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C5" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="28" t="s">
+      <c r="D5" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="29"/>
+      <c r="E5" s="30"/>
       <c r="H5" s="18" t="s">
         <v>22</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="23" t="s">
+      <c r="D6" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="E6" s="23"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E6" s="24"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="23" t="s">
+      <c r="D7" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="E7" s="23"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E7" s="24"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -1079,7 +1079,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -1093,7 +1093,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
@@ -1108,7 +1108,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B25" si="0">B11+1</f>
         <v>3</v>
@@ -1121,7 +1121,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1134,7 +1134,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1143,7 +1143,7 @@
       <c r="D14" s="1"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1152,7 +1152,7 @@
       <c r="D15" s="1"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1161,7 +1161,7 @@
       <c r="D16" s="1"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1170,7 +1170,7 @@
       <c r="D17" s="1"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1179,7 +1179,7 @@
       <c r="D18" s="3"/>
       <c r="E18" s="16"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1188,7 +1188,7 @@
       <c r="D19" s="3"/>
       <c r="E19" s="16"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1197,7 +1197,7 @@
       <c r="D20" s="3"/>
       <c r="E20" s="16"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1206,7 +1206,7 @@
       <c r="D21" s="3"/>
       <c r="E21" s="16"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1215,7 +1215,7 @@
       <c r="D22" s="3"/>
       <c r="E22" s="16"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1224,7 +1224,7 @@
       <c r="D23" s="3"/>
       <c r="E23" s="16"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1233,7 +1233,7 @@
       <c r="D24" s="3"/>
       <c r="E24" s="16"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1242,10 +1242,10 @@
       <c r="D25" s="3"/>
       <c r="E25" s="16"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E26" s="11"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C27" s="12" t="s">
         <v>8</v>
       </c>
@@ -1275,39 +1275,39 @@
   </sheetPr>
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:J1"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="6"/>
-    <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
-    <col min="3" max="4" width="16.33203125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="41.44140625" style="6" customWidth="1"/>
-    <col min="6" max="8" width="8.88671875" style="6"/>
+    <col min="1" max="1" width="8.85546875" style="6"/>
+    <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
+    <col min="3" max="4" width="16.28515625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="41.42578125" style="6" customWidth="1"/>
+    <col min="6" max="8" width="8.85546875" style="6"/>
     <col min="9" max="9" width="22" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="6"/>
+    <col min="10" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="30" t="s">
+      <c r="H1" s="31" t="s">
         <v>50</v>
       </c>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B2" s="26" t="s">
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B2" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
       <c r="H2" s="3"/>
       <c r="I2" s="20" t="s">
         <v>30</v>
@@ -1316,7 +1316,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H3" s="18" t="s">
         <v>20</v>
       </c>
@@ -1327,14 +1327,14 @@
         <v>236</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="31" t="s">
+      <c r="D4" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="31"/>
+      <c r="E4" s="32"/>
       <c r="H4" s="18" t="s">
         <v>21</v>
       </c>
@@ -1345,40 +1345,40 @@
         <v>236</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="32" t="s">
+      <c r="D5" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="33"/>
+      <c r="E5" s="34"/>
       <c r="H5" s="18" t="s">
         <v>22</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="23" t="s">
+      <c r="D6" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="E6" s="23"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E6" s="24"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="23" t="s">
+      <c r="D7" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="E7" s="23"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E7" s="24"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -1392,7 +1392,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -1404,7 +1404,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
@@ -1417,7 +1417,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B26" si="0">B11+1</f>
         <v>3</v>
@@ -1430,7 +1430,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1443,7 +1443,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1456,7 +1456,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1465,7 +1465,7 @@
       <c r="D15" s="1"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1474,7 +1474,7 @@
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1483,7 +1483,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1492,7 +1492,7 @@
       <c r="D18" s="1"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1501,7 +1501,7 @@
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1510,7 +1510,7 @@
       <c r="D20" s="1"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1519,7 +1519,7 @@
       <c r="D21" s="1"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1528,7 +1528,7 @@
       <c r="D22" s="1"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1537,7 +1537,7 @@
       <c r="D23" s="1"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1546,7 +1546,7 @@
       <c r="D24" s="1"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1555,7 +1555,7 @@
       <c r="D25" s="1"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1564,15 +1564,17 @@
       <c r="D26" s="1"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E27" s="11"/>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C28" s="12" t="s">
         <v>8</v>
       </c>
       <c r="D28" s="13"/>
-      <c r="E28" s="1"/>
+      <c r="E28" s="1">
+        <v>0.5</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1595,41 +1597,41 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="6"/>
-    <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" style="6" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="6"/>
+    <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" style="6" customWidth="1"/>
     <col min="4" max="4" width="25" style="6" customWidth="1"/>
-    <col min="5" max="5" width="41.44140625" style="6" customWidth="1"/>
-    <col min="6" max="6" width="37.6640625" style="6" customWidth="1"/>
-    <col min="7" max="8" width="8.88671875" style="6"/>
-    <col min="9" max="9" width="26.6640625" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="6"/>
+    <col min="5" max="5" width="41.42578125" style="6" customWidth="1"/>
+    <col min="6" max="6" width="37.7109375" style="6" customWidth="1"/>
+    <col min="7" max="8" width="8.85546875" style="6"/>
+    <col min="9" max="9" width="26.7109375" style="6" customWidth="1"/>
+    <col min="10" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="30" t="s">
+      <c r="H1" s="31" t="s">
         <v>50</v>
       </c>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B2" s="26" t="s">
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B2" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
       <c r="H2" s="3"/>
       <c r="I2" s="20" t="s">
         <v>30</v>
@@ -1638,7 +1640,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H3" s="18" t="s">
         <v>20</v>
       </c>
@@ -1649,14 +1651,14 @@
         <v>236</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C4" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="34" t="s">
+      <c r="D4" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="34"/>
+      <c r="E4" s="35"/>
       <c r="H4" s="18" t="s">
         <v>21</v>
       </c>
@@ -1667,40 +1669,40 @@
         <v>236</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C5" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="35" t="s">
+      <c r="D5" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="36"/>
+      <c r="E5" s="37"/>
       <c r="H5" s="18" t="s">
         <v>22</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="23" t="s">
+      <c r="D6" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="E6" s="23"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E6" s="24"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="23" t="s">
+      <c r="D7" s="24" t="s">
         <v>87</v>
       </c>
-      <c r="E7" s="23"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E7" s="24"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -1714,7 +1716,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -1728,110 +1730,110 @@
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="39" t="s">
+      <c r="C11" s="23" t="s">
         <v>93</v>
       </c>
-      <c r="D11" s="39" t="s">
+      <c r="D11" s="23" t="s">
         <v>94</v>
       </c>
-      <c r="E11" s="39" t="s">
+      <c r="E11" s="23" t="s">
         <v>98</v>
       </c>
       <c r="F11" s="22"/>
     </row>
-    <row r="12" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="150" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="39" t="s">
+      <c r="C12" s="23" t="s">
         <v>93</v>
       </c>
-      <c r="D12" s="39" t="s">
+      <c r="D12" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="E12" s="39" t="s">
+      <c r="E12" s="23" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="150" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C13" s="39" t="s">
+      <c r="C13" s="23" t="s">
         <v>93</v>
       </c>
-      <c r="D13" s="39" t="s">
+      <c r="D13" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="E13" s="39" t="s">
+      <c r="E13" s="23" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C14" s="39" t="s">
+      <c r="C14" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="D14" s="39" t="s">
+      <c r="D14" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="E14" s="39" t="s">
+      <c r="E14" s="23" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C15" s="39" t="s">
+      <c r="C15" s="23" t="s">
         <v>93</v>
       </c>
-      <c r="D15" s="39" t="s">
+      <c r="D15" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="E15" s="39" t="s">
+      <c r="E15" s="23" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C16" s="39"/>
-      <c r="D16" s="39"/>
-      <c r="E16" s="39"/>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C16" s="23"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C17" s="39"/>
-      <c r="D17" s="39"/>
-      <c r="E17" s="39"/>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C17" s="23"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="23"/>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C18" s="39"/>
-      <c r="D18" s="39"/>
-      <c r="E18" s="39"/>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C18" s="23"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1840,7 +1842,7 @@
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1849,7 +1851,7 @@
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1858,7 +1860,7 @@
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1867,7 +1869,7 @@
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1876,7 +1878,7 @@
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1885,7 +1887,7 @@
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1894,7 +1896,7 @@
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1903,7 +1905,7 @@
       <c r="D26" s="1"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" s="3">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1912,7 +1914,7 @@
       <c r="D27" s="2"/>
       <c r="E27" s="1"/>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" s="3">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1921,7 +1923,7 @@
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" s="3">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1930,7 +1932,7 @@
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" s="3">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1939,16 +1941,16 @@
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E31" s="11"/>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C32" s="12" t="s">
         <v>8</v>
       </c>
       <c r="D32" s="13"/>
       <c r="E32" s="1">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1972,41 +1974,41 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="6"/>
-    <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" style="6" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="6"/>
+    <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" style="6" customWidth="1"/>
     <col min="4" max="4" width="18" style="6" customWidth="1"/>
     <col min="5" max="5" width="24" style="6" customWidth="1"/>
-    <col min="6" max="6" width="16.6640625" style="6" customWidth="1"/>
-    <col min="7" max="8" width="8.88671875" style="6"/>
-    <col min="9" max="9" width="26.6640625" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="6"/>
+    <col min="6" max="6" width="16.7109375" style="6" customWidth="1"/>
+    <col min="7" max="8" width="8.85546875" style="6"/>
+    <col min="9" max="9" width="26.7109375" style="6" customWidth="1"/>
+    <col min="10" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="30" t="s">
+      <c r="H1" s="31" t="s">
         <v>50</v>
       </c>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B2" s="26" t="s">
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B2" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
       <c r="H2" s="3"/>
       <c r="I2" s="20" t="s">
         <v>30</v>
@@ -2015,7 +2017,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H3" s="18" t="s">
         <v>20</v>
       </c>
@@ -2026,12 +2028,12 @@
         <v>236</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C4" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
       <c r="H4" s="18" t="s">
         <v>21</v>
       </c>
@@ -2042,31 +2044,31 @@
         <v>236</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="23" t="s">
+      <c r="D5" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="E5" s="23"/>
+      <c r="E5" s="24"/>
       <c r="H5" s="18" t="s">
         <v>22</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="23" t="s">
+      <c r="D6" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="E6" s="23"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E6" s="24"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -2083,7 +2085,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -2100,7 +2102,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
@@ -2118,7 +2120,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
@@ -2136,7 +2138,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -2154,7 +2156,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -2172,7 +2174,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -2190,7 +2192,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -2208,7 +2210,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -2218,7 +2220,7 @@
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -2228,7 +2230,7 @@
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -2238,7 +2240,7 @@
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -2248,7 +2250,7 @@
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -2258,7 +2260,7 @@
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -2268,7 +2270,7 @@
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -2278,7 +2280,7 @@
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -2288,7 +2290,7 @@
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -2298,7 +2300,7 @@
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -2308,7 +2310,7 @@
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27" s="3">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -2318,7 +2320,7 @@
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28" s="3">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -2328,7 +2330,7 @@
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B29" s="3">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -2338,7 +2340,7 @@
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B30" s="3">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -2348,15 +2350,15 @@
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E31" s="11"/>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C32" s="37" t="s">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C32" s="38" t="s">
         <v>79</v>
       </c>
-      <c r="D32" s="38"/>
-      <c r="E32" s="38"/>
+      <c r="D32" s="39"/>
+      <c r="E32" s="39"/>
       <c r="F32" s="19"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added error if repo file does not exist + Finished Review + Rename Diagram
</commit_message>
<xml_diff>
--- a/Docs/Lab01/Lab01_ReviewReport.xlsx
+++ b/Docs/Lab01/Lab01_ReviewReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rusu1\Desktop\VVSS\VVSS\Docs\Lab01\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pigeon\Documents\facultate\An3\VVSS\Inventory\Docs\Lab01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBAB1658-9E99-46AA-A26D-F8A649D2D19B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D976A8D-D4D1-43C0-83C5-CF9CC8BE6919}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Coding Phase Defects" sheetId="5" r:id="rId3"/>
     <sheet name="DynamicCodeAnalysis" sheetId="8" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -567,6 +567,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -614,9 +617,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -961,40 +961,40 @@
   </sheetPr>
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="6"/>
-    <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
-    <col min="3" max="4" width="16.33203125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="41.44140625" style="6" customWidth="1"/>
-    <col min="6" max="8" width="8.88671875" style="6"/>
+    <col min="1" max="1" width="8.85546875" style="6"/>
+    <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
+    <col min="3" max="4" width="16.28515625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="41.42578125" style="6" customWidth="1"/>
+    <col min="6" max="8" width="8.85546875" style="6"/>
     <col min="9" max="9" width="21" style="6" customWidth="1"/>
-    <col min="10" max="10" width="14.44140625" style="6" customWidth="1"/>
-    <col min="11" max="16384" width="8.88671875" style="6"/>
+    <col min="10" max="10" width="14.42578125" style="6" customWidth="1"/>
+    <col min="11" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="24" t="s">
+      <c r="H1" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B2" s="26" t="s">
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B2" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
       <c r="H2" s="3"/>
       <c r="I2" s="20" t="s">
         <v>30</v>
@@ -1003,7 +1003,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H3" s="18" t="s">
         <v>20</v>
       </c>
@@ -1014,14 +1014,14 @@
         <v>236</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C4" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="27" t="s">
+      <c r="D4" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="27"/>
+      <c r="E4" s="28"/>
       <c r="H4" s="18" t="s">
         <v>21</v>
       </c>
@@ -1032,40 +1032,40 @@
         <v>236</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C5" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="28" t="s">
+      <c r="D5" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="29"/>
+      <c r="E5" s="30"/>
       <c r="H5" s="18" t="s">
         <v>22</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="23" t="s">
+      <c r="D6" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="E6" s="23"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E6" s="24"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="23" t="s">
+      <c r="D7" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="E7" s="23"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E7" s="24"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -1079,7 +1079,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -1093,7 +1093,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
@@ -1108,7 +1108,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B25" si="0">B11+1</f>
         <v>3</v>
@@ -1121,7 +1121,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1134,7 +1134,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1143,7 +1143,7 @@
       <c r="D14" s="1"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1152,7 +1152,7 @@
       <c r="D15" s="1"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1161,7 +1161,7 @@
       <c r="D16" s="1"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1170,7 +1170,7 @@
       <c r="D17" s="1"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1179,7 +1179,7 @@
       <c r="D18" s="3"/>
       <c r="E18" s="16"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1188,7 +1188,7 @@
       <c r="D19" s="3"/>
       <c r="E19" s="16"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1197,7 +1197,7 @@
       <c r="D20" s="3"/>
       <c r="E20" s="16"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1206,7 +1206,7 @@
       <c r="D21" s="3"/>
       <c r="E21" s="16"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1215,7 +1215,7 @@
       <c r="D22" s="3"/>
       <c r="E22" s="16"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1224,7 +1224,7 @@
       <c r="D23" s="3"/>
       <c r="E23" s="16"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1233,7 +1233,7 @@
       <c r="D24" s="3"/>
       <c r="E24" s="16"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1242,10 +1242,10 @@
       <c r="D25" s="3"/>
       <c r="E25" s="16"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E26" s="11"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C27" s="12" t="s">
         <v>8</v>
       </c>
@@ -1275,39 +1275,39 @@
   </sheetPr>
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:J1"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="6"/>
-    <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
-    <col min="3" max="4" width="16.33203125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="41.44140625" style="6" customWidth="1"/>
-    <col min="6" max="8" width="8.88671875" style="6"/>
+    <col min="1" max="1" width="8.85546875" style="6"/>
+    <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
+    <col min="3" max="4" width="16.28515625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="41.42578125" style="6" customWidth="1"/>
+    <col min="6" max="8" width="8.85546875" style="6"/>
     <col min="9" max="9" width="22" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="6"/>
+    <col min="10" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="30" t="s">
+      <c r="H1" s="31" t="s">
         <v>50</v>
       </c>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B2" s="26" t="s">
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B2" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
       <c r="H2" s="3"/>
       <c r="I2" s="20" t="s">
         <v>30</v>
@@ -1316,7 +1316,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H3" s="18" t="s">
         <v>20</v>
       </c>
@@ -1327,14 +1327,14 @@
         <v>236</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="31" t="s">
+      <c r="D4" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="31"/>
+      <c r="E4" s="32"/>
       <c r="H4" s="18" t="s">
         <v>21</v>
       </c>
@@ -1345,40 +1345,40 @@
         <v>236</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="32" t="s">
+      <c r="D5" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="33"/>
+      <c r="E5" s="34"/>
       <c r="H5" s="18" t="s">
         <v>22</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="23" t="s">
+      <c r="D6" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="E6" s="23"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E6" s="24"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="23" t="s">
+      <c r="D7" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="E7" s="23"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E7" s="24"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -1392,7 +1392,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -1404,7 +1404,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
@@ -1417,7 +1417,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B26" si="0">B11+1</f>
         <v>3</v>
@@ -1430,7 +1430,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1443,7 +1443,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1456,7 +1456,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1465,7 +1465,7 @@
       <c r="D15" s="1"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1474,7 +1474,7 @@
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1483,7 +1483,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1492,7 +1492,7 @@
       <c r="D18" s="1"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1501,7 +1501,7 @@
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1510,7 +1510,7 @@
       <c r="D20" s="1"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1519,7 +1519,7 @@
       <c r="D21" s="1"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1528,7 +1528,7 @@
       <c r="D22" s="1"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1537,7 +1537,7 @@
       <c r="D23" s="1"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1546,7 +1546,7 @@
       <c r="D24" s="1"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1555,7 +1555,7 @@
       <c r="D25" s="1"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1564,15 +1564,17 @@
       <c r="D26" s="1"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E27" s="11"/>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C28" s="12" t="s">
         <v>8</v>
       </c>
       <c r="D28" s="13"/>
-      <c r="E28" s="1"/>
+      <c r="E28" s="1">
+        <v>0.5</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1595,41 +1597,41 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="6"/>
-    <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" style="6" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="6"/>
+    <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" style="6" customWidth="1"/>
     <col min="4" max="4" width="25" style="6" customWidth="1"/>
-    <col min="5" max="5" width="41.44140625" style="6" customWidth="1"/>
-    <col min="6" max="6" width="37.6640625" style="6" customWidth="1"/>
-    <col min="7" max="8" width="8.88671875" style="6"/>
-    <col min="9" max="9" width="26.6640625" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="6"/>
+    <col min="5" max="5" width="41.42578125" style="6" customWidth="1"/>
+    <col min="6" max="6" width="37.7109375" style="6" customWidth="1"/>
+    <col min="7" max="8" width="8.85546875" style="6"/>
+    <col min="9" max="9" width="26.7109375" style="6" customWidth="1"/>
+    <col min="10" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="30" t="s">
+      <c r="H1" s="31" t="s">
         <v>50</v>
       </c>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B2" s="26" t="s">
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B2" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
       <c r="H2" s="3"/>
       <c r="I2" s="20" t="s">
         <v>30</v>
@@ -1638,7 +1640,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H3" s="18" t="s">
         <v>20</v>
       </c>
@@ -1649,14 +1651,14 @@
         <v>236</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C4" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="34" t="s">
+      <c r="D4" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="34"/>
+      <c r="E4" s="35"/>
       <c r="H4" s="18" t="s">
         <v>21</v>
       </c>
@@ -1667,40 +1669,40 @@
         <v>236</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C5" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="35" t="s">
+      <c r="D5" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="36"/>
+      <c r="E5" s="37"/>
       <c r="H5" s="18" t="s">
         <v>22</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="23" t="s">
+      <c r="D6" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="E6" s="23"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E6" s="24"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="23" t="s">
+      <c r="D7" s="24" t="s">
         <v>87</v>
       </c>
-      <c r="E7" s="23"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E7" s="24"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -1714,7 +1716,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -1728,110 +1730,110 @@
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="39" t="s">
+      <c r="C11" s="23" t="s">
         <v>93</v>
       </c>
-      <c r="D11" s="39" t="s">
+      <c r="D11" s="23" t="s">
         <v>94</v>
       </c>
-      <c r="E11" s="39" t="s">
+      <c r="E11" s="23" t="s">
         <v>98</v>
       </c>
       <c r="F11" s="22"/>
     </row>
-    <row r="12" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="150" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="39" t="s">
+      <c r="C12" s="23" t="s">
         <v>93</v>
       </c>
-      <c r="D12" s="39" t="s">
+      <c r="D12" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="E12" s="39" t="s">
+      <c r="E12" s="23" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="150" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C13" s="39" t="s">
+      <c r="C13" s="23" t="s">
         <v>93</v>
       </c>
-      <c r="D13" s="39" t="s">
+      <c r="D13" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="E13" s="39" t="s">
+      <c r="E13" s="23" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C14" s="39" t="s">
+      <c r="C14" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="D14" s="39" t="s">
+      <c r="D14" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="E14" s="39" t="s">
+      <c r="E14" s="23" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C15" s="39" t="s">
+      <c r="C15" s="23" t="s">
         <v>93</v>
       </c>
-      <c r="D15" s="39" t="s">
+      <c r="D15" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="E15" s="39" t="s">
+      <c r="E15" s="23" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C16" s="39"/>
-      <c r="D16" s="39"/>
-      <c r="E16" s="39"/>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C16" s="23"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C17" s="39"/>
-      <c r="D17" s="39"/>
-      <c r="E17" s="39"/>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C17" s="23"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="23"/>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C18" s="39"/>
-      <c r="D18" s="39"/>
-      <c r="E18" s="39"/>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C18" s="23"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1840,7 +1842,7 @@
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1849,7 +1851,7 @@
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1858,7 +1860,7 @@
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1867,7 +1869,7 @@
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1876,7 +1878,7 @@
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1885,7 +1887,7 @@
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1894,7 +1896,7 @@
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1903,7 +1905,7 @@
       <c r="D26" s="1"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" s="3">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1912,7 +1914,7 @@
       <c r="D27" s="2"/>
       <c r="E27" s="1"/>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" s="3">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1921,7 +1923,7 @@
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" s="3">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1930,7 +1932,7 @@
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" s="3">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1939,16 +1941,16 @@
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E31" s="11"/>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C32" s="12" t="s">
         <v>8</v>
       </c>
       <c r="D32" s="13"/>
       <c r="E32" s="1">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1972,41 +1974,41 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="6"/>
-    <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" style="6" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="6"/>
+    <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" style="6" customWidth="1"/>
     <col min="4" max="4" width="18" style="6" customWidth="1"/>
     <col min="5" max="5" width="24" style="6" customWidth="1"/>
-    <col min="6" max="6" width="16.6640625" style="6" customWidth="1"/>
-    <col min="7" max="8" width="8.88671875" style="6"/>
-    <col min="9" max="9" width="26.6640625" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="6"/>
+    <col min="6" max="6" width="16.7109375" style="6" customWidth="1"/>
+    <col min="7" max="8" width="8.85546875" style="6"/>
+    <col min="9" max="9" width="26.7109375" style="6" customWidth="1"/>
+    <col min="10" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="30" t="s">
+      <c r="H1" s="31" t="s">
         <v>50</v>
       </c>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B2" s="26" t="s">
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B2" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
       <c r="H2" s="3"/>
       <c r="I2" s="20" t="s">
         <v>30</v>
@@ -2015,7 +2017,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H3" s="18" t="s">
         <v>20</v>
       </c>
@@ -2026,12 +2028,12 @@
         <v>236</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C4" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
       <c r="H4" s="18" t="s">
         <v>21</v>
       </c>
@@ -2042,31 +2044,31 @@
         <v>236</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="23" t="s">
+      <c r="D5" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="E5" s="23"/>
+      <c r="E5" s="24"/>
       <c r="H5" s="18" t="s">
         <v>22</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="23" t="s">
+      <c r="D6" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="E6" s="23"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E6" s="24"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -2083,7 +2085,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -2100,7 +2102,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
@@ -2118,7 +2120,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
@@ -2136,7 +2138,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -2154,7 +2156,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -2172,7 +2174,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -2190,7 +2192,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -2208,7 +2210,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -2218,7 +2220,7 @@
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -2228,7 +2230,7 @@
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -2238,7 +2240,7 @@
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -2248,7 +2250,7 @@
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -2258,7 +2260,7 @@
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -2268,7 +2270,7 @@
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -2278,7 +2280,7 @@
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -2288,7 +2290,7 @@
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -2298,7 +2300,7 @@
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -2308,7 +2310,7 @@
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27" s="3">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -2318,7 +2320,7 @@
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28" s="3">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -2328,7 +2330,7 @@
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B29" s="3">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -2338,7 +2340,7 @@
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B30" s="3">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -2348,15 +2350,15 @@
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E31" s="11"/>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C32" s="37" t="s">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C32" s="38" t="s">
         <v>79</v>
       </c>
-      <c r="D32" s="38"/>
-      <c r="E32" s="38"/>
+      <c r="D32" s="39"/>
+      <c r="E32" s="39"/>
       <c r="F32" s="19"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Tests for Add Part
</commit_message>
<xml_diff>
--- a/Docs/Lab01/Lab01_ReviewReport.xlsx
+++ b/Docs/Lab01/Lab01_ReviewReport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pigeon\Documents\facultate\An3\VVSS\Inventory\Docs\Lab01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D976A8D-D4D1-43C0-83C5-CF9CC8BE6919}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{123CBEBD-CEF6-4C19-92F0-38D84218A469}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="650" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -168,9 +168,6 @@
     <t>A09</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t xml:space="preserve">Nu există Validator. Ar trebui adăugate clase de validare pentru piesă și pentru produs. </t>
   </si>
   <si>
@@ -328,6 +325,9 @@
   </si>
   <si>
     <t>La operațiile de modificare și ștergere, în interfața cu utilizatorul ar trebui să apară un mesaj prin care să fie atenționat că este necesar să selecteze un obiect, in momentul de față, dacă un obiect nu e selectat, valoarea va fi null si se continua cu null în funcțiile urmatoare.</t>
+  </si>
+  <si>
+    <t>A07</t>
   </si>
 </sst>
 </file>
@@ -961,7 +961,7 @@
   </sheetPr>
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
@@ -983,7 +983,7 @@
         <v>3</v>
       </c>
       <c r="H1" s="25" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I1" s="26"/>
       <c r="J1" s="26"/>
@@ -1052,7 +1052,7 @@
         <v>2</v>
       </c>
       <c r="D6" s="24" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E6" s="24"/>
     </row>
@@ -1061,7 +1061,7 @@
         <v>1</v>
       </c>
       <c r="D7" s="24" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E7" s="24"/>
     </row>
@@ -1131,7 +1131,7 @@
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -1275,8 +1275,8 @@
   </sheetPr>
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1296,7 +1296,7 @@
         <v>3</v>
       </c>
       <c r="H1" s="31" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I1" s="26"/>
       <c r="J1" s="26"/>
@@ -1365,7 +1365,7 @@
         <v>2</v>
       </c>
       <c r="D6" s="24" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E6" s="24"/>
     </row>
@@ -1374,7 +1374,7 @@
         <v>1</v>
       </c>
       <c r="D7" s="24" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E7" s="24"/>
     </row>
@@ -1401,7 +1401,7 @@
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -1414,7 +1414,7 @@
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1427,7 +1427,7 @@
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -1436,11 +1436,11 @@
         <v>4</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>45</v>
+        <v>98</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -1453,7 +1453,7 @@
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -1597,8 +1597,8 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1620,7 +1620,7 @@
         <v>3</v>
       </c>
       <c r="H1" s="31" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I1" s="26"/>
       <c r="J1" s="26"/>
@@ -1689,7 +1689,7 @@
         <v>2</v>
       </c>
       <c r="D6" s="24" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E6" s="24"/>
     </row>
@@ -1698,7 +1698,7 @@
         <v>1</v>
       </c>
       <c r="D7" s="24" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E7" s="24"/>
     </row>
@@ -1721,13 +1721,13 @@
         <v>1</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -1736,13 +1736,13 @@
         <v>2</v>
       </c>
       <c r="C11" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="D11" s="23" t="s">
         <v>93</v>
       </c>
-      <c r="D11" s="23" t="s">
-        <v>94</v>
-      </c>
       <c r="E11" s="23" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F11" s="22"/>
     </row>
@@ -1752,13 +1752,13 @@
         <v>3</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D12" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="E12" s="23" t="s">
         <v>85</v>
-      </c>
-      <c r="E12" s="23" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="150" x14ac:dyDescent="0.25">
@@ -1767,13 +1767,13 @@
         <v>4</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D13" s="23" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E13" s="23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1782,13 +1782,13 @@
         <v>5</v>
       </c>
       <c r="C14" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="D14" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="D14" s="23" t="s">
-        <v>90</v>
-      </c>
       <c r="E14" s="23" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -1797,13 +1797,13 @@
         <v>6</v>
       </c>
       <c r="C15" s="23" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D15" s="23" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E15" s="23" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -1997,7 +1997,7 @@
         <v>3</v>
       </c>
       <c r="H1" s="31" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I1" s="26"/>
       <c r="J1" s="26"/>
@@ -2049,7 +2049,7 @@
         <v>2</v>
       </c>
       <c r="D5" s="24" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E5" s="24"/>
       <c r="H5" s="18" t="s">
@@ -2064,7 +2064,7 @@
         <v>1</v>
       </c>
       <c r="D6" s="24" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E6" s="24"/>
     </row>
@@ -2090,16 +2090,16 @@
         <v>1</v>
       </c>
       <c r="C10" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="F10" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2108,16 +2108,16 @@
         <v>2</v>
       </c>
       <c r="C11" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="E11" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="F11" s="2" t="s">
         <v>60</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -2126,16 +2126,16 @@
         <v>3</v>
       </c>
       <c r="C12" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="E12" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="F12" s="2" t="s">
         <v>64</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2144,16 +2144,16 @@
         <v>4</v>
       </c>
       <c r="C13" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="E13" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="F13" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -2162,16 +2162,16 @@
         <v>5</v>
       </c>
       <c r="C14" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="E14" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F14" s="2" t="s">
         <v>71</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2180,16 +2180,16 @@
         <v>6</v>
       </c>
       <c r="C15" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="E15" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="F15" s="2" t="s">
         <v>75</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -2198,16 +2198,16 @@
         <v>7</v>
       </c>
       <c r="C16" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="E16" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F16" s="2" t="s">
         <v>81</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
@@ -2355,7 +2355,7 @@
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C32" s="38" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D32" s="39"/>
       <c r="E32" s="39"/>

</xml_diff>